<commit_message>
Added data for GDP and employments for RES
</commit_message>
<xml_diff>
--- a/import/raw_data/id_primary_energy_carrier.xlsx
+++ b/import/raw_data/id_primary_energy_carrier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bef\GitHub\micat\import\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D109318E-D6A7-46D4-AEDF-E18702B784F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D26DAB-8DC7-4093-9A8B-0269AEA9F0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27876" yWindow="2928" windowWidth="14400" windowHeight="8172" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6048" yWindow="1728" windowWidth="46080" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,10 +77,10 @@
     <t>Electricity</t>
   </si>
   <si>
-    <t>Electricity (for heat and hydrogen/synthetic fuel production)</t>
-  </si>
-  <si>
     <t>Other (incl. nuclear)</t>
+  </si>
+  <si>
+    <t>Electricity (for heat and hydrogen / e-fuel production)</t>
   </si>
 </sst>
 </file>
@@ -419,19 +419,19 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="3" max="3" width="51.81640625" customWidth="1"/>
-    <col min="7" max="7" width="36.7265625" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="51.77734375" customWidth="1"/>
+    <col min="7" max="7" width="36.77734375" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -442,7 +442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -453,7 +453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -464,7 +464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -475,7 +475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -486,7 +486,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -498,7 +498,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -506,13 +506,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1"/>
       <c r="O7" s="1"/>
       <c r="S7" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -520,7 +520,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -541,15 +541,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010081027A5C4AB68A40A5017F28CDCC410C" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="f1f428d4bdb6f67b400b210b48125618">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ca47701c-f272-4f81-9665-1c7dbebc0776" xmlns:ns3="89bcd336-abeb-4a08-b6b9-8f1906e00f8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8189f6f0f7c839d9d0d3622fd62ec189" ns2:_="" ns3:_="">
     <xsd:import namespace="ca47701c-f272-4f81-9665-1c7dbebc0776"/>
@@ -802,6 +793,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52125EBF-9B68-45F0-8CEC-88F715CB1D25}">
   <ds:schemaRefs>
@@ -820,14 +820,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12901B2F-7E3B-4BCF-B2FA-01331DEC9CC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF80A771-499D-474A-AF97-0816FB3172DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -844,4 +836,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12901B2F-7E3B-4BCF-B2FA-01331DEC9CC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>